<commit_message>
updated risk descriptions and contect with if/then format
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34658
</commit_message>
<xml_diff>
--- a/Project Management/eCL OY4/CCO OY4_eCoaching Log Risk Register.xlsx
+++ b/Project Management/eCL OY4/CCO OY4_eCoaching Log Risk Register.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Project Management\eCL OY4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485"/>
   </bookViews>
@@ -14,7 +19,7 @@
     <definedName name="owssvr_2" localSheetId="0" hidden="1">'Integrated Register'!$A$3:$V$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Integrated Register'!$A$1:$V$37</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
   <si>
     <t>Status</t>
   </si>
@@ -209,9 +214,6 @@
 Risk is Closed 7/30/14</t>
   </si>
   <si>
-    <t>Engineers supporting multiple projects will have negative impact on delivery of eCL changes</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
@@ -266,9 +268,6 @@
     <t>Open</t>
   </si>
   <si>
-    <t>Application will not work</t>
-  </si>
-  <si>
     <t>Closed row 12; added two new risks</t>
   </si>
   <si>
@@ -293,34 +292,19 @@
     <t>Closed row 13</t>
   </si>
   <si>
-    <t>Incomplete and inaccurate data in centralized CCO CSR/Employee database (eWFM/People Soft) - creates inconsistencies in records being created from external sources (quality control system) compared to records created directly in eCL.</t>
-  </si>
-  <si>
     <t>Resources are supporting other engineering projects</t>
   </si>
   <si>
     <t>Mike</t>
   </si>
   <si>
-    <t>File share access changing without warning. This occurred on 1/16/2016</t>
-  </si>
-  <si>
     <t>individuals identified in OY3/OY4 will be more aligned with the project</t>
   </si>
   <si>
     <t>work being delayed</t>
   </si>
   <si>
-    <t>Rely on HR to make HR Job Code updates in their system.  We are low priority for them</t>
-  </si>
-  <si>
     <t>HR Job Code change dependences in the eCL system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job Code changes are not communicated and the eCL system requires modifications to function properly </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> delay of feed updates impact our delivery time for eCL system updates</t>
   </si>
   <si>
     <t>Total Impact on occurrence
@@ -352,6 +336,30 @@
   </si>
   <si>
     <t>Updated in accurate data, engineering resource risk and file share risks.  Added 2 new risks related to Job Code changes</t>
+  </si>
+  <si>
+    <t>If the data in centralized CCO CSR/Employee database (eWFM/People Soft) is incomplete or inaccurate it will create inconsistencies in records being created from external sources (quality control system) compared to records created directly in eCL.</t>
+  </si>
+  <si>
+    <t>If engineers are supporting multiple projects it will have negative impact on delivery of eCL changes.</t>
+  </si>
+  <si>
+    <t>If file share access changes without warning the application will not work.</t>
+  </si>
+  <si>
+    <t>This occurred on 1/16/2016</t>
+  </si>
+  <si>
+    <t>Modified discriptions and context of open risks to If/Then type format (Doug Stearns)</t>
+  </si>
+  <si>
+    <t>If HR Job Codes change and are not communicated the eCL system will be unavailable to HR until modifications are made.</t>
+  </si>
+  <si>
+    <t>Rely on HR to make HR Job Code updates in their system.  We are low priority for them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If HR does not make HR Job Code updates in their system in a timely manner a delay in feed updates will impact time for eCL system updates. </t>
   </si>
 </sst>
 </file>
@@ -1189,6 +1197,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1314,7 +1325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1349,7 +1360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1563,8 +1574,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1631,7 @@
     </row>
     <row r="2" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -1658,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2</v>
@@ -1682,7 +1693,7 @@
         <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>21</v>
@@ -1714,7 +1725,7 @@
     </row>
     <row r="4" spans="1:22" ht="113.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
@@ -1842,19 +1853,19 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D6" s="7">
         <v>41108</v>
       </c>
       <c r="E6" s="7">
-        <v>42403</v>
+        <v>42551</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>25</v>
@@ -1960,13 +1971,13 @@
         <v>48</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
@@ -2109,7 +2120,7 @@
         <v>42058</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
@@ -2146,7 +2157,7 @@
       <c r="S10" s="9"/>
       <c r="T10" s="5"/>
       <c r="U10" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="V10" s="9"/>
     </row>
@@ -2156,25 +2167,25 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="D11" s="9">
         <v>41850</v>
       </c>
       <c r="E11" s="9">
-        <v>42403</v>
+        <v>42551</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>27</v>
@@ -2200,17 +2211,17 @@
       </c>
       <c r="P11" s="15"/>
       <c r="Q11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R11" s="9">
         <v>41850</v>
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="V11" s="9"/>
     </row>
@@ -2220,7 +2231,7 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="9">
         <v>42060</v>
@@ -2229,16 +2240,16 @@
         <v>42137</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>27</v>
@@ -2264,27 +2275,27 @@
       </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R12" s="9">
         <v>42064</v>
       </c>
       <c r="S12" s="9"/>
       <c r="T12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="U12" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="V12" s="9"/>
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="9">
         <v>42137</v>
@@ -2293,16 +2304,16 @@
         <v>42270</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>27</v>
@@ -2328,45 +2339,45 @@
       </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R13" s="9">
         <v>42142</v>
       </c>
       <c r="S13" s="9"/>
       <c r="T13" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="V13" s="9"/>
     </row>
     <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D14" s="9">
         <v>42137</v>
       </c>
       <c r="E14" s="9">
-        <v>42403</v>
+        <v>42551</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>27</v>
@@ -2392,43 +2403,45 @@
       </c>
       <c r="P14" s="15"/>
       <c r="Q14" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R14" s="9">
         <v>42142</v>
       </c>
       <c r="S14" s="9"/>
       <c r="T14" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="V14" s="9"/>
     </row>
     <row r="15" spans="1:22" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="4" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D15" s="9">
         <v>42038</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="9">
+        <v>42551</v>
+      </c>
       <c r="F15" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>27</v>
@@ -2454,43 +2467,45 @@
       </c>
       <c r="P15" s="15"/>
       <c r="Q15" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="R15" s="9">
         <v>42403</v>
       </c>
       <c r="S15" s="9"/>
       <c r="T15" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="V15" s="9"/>
     </row>
     <row r="16" spans="1:22" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="4" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="D16" s="9">
         <v>42403</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="9">
+        <v>42551</v>
+      </c>
       <c r="F16" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>27</v>
@@ -2516,17 +2531,17 @@
       </c>
       <c r="P16" s="15"/>
       <c r="Q16" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="R16" s="9">
         <v>42403</v>
       </c>
       <c r="S16" s="9"/>
       <c r="T16" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="V16" s="9"/>
     </row>
@@ -3334,7 +3349,7 @@
     <mergeCell ref="A2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="17" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LVangent Proprietary Information</oddFooter>
   </headerFooter>
@@ -3346,10 +3361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3362,7 +3377,7 @@
         <v>42060</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3370,7 +3385,7 @@
         <v>42088</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3378,7 +3393,7 @@
         <v>42096</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3386,7 +3401,7 @@
         <v>42137</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3394,7 +3409,7 @@
         <v>42270</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3402,7 +3417,15 @@
         <v>42403</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>42551</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3411,21 +3434,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5C6E04F5F2CA4DBF07DC2DA055DA5A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b67af60ff7fc8b8e5184fdb460baaf96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3539,17 +3547,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3563,17 +3587,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Closed HR related risks
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34697
</commit_message>
<xml_diff>
--- a/Project Management/eCL OY4/CCO OY4_eCoaching Log Risk Register.xlsx
+++ b/Project Management/eCL OY4/CCO OY4_eCoaching Log Risk Register.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Project Management\eCL OY4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Integrated Register" sheetId="2" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <definedName name="owssvr_2" localSheetId="0" hidden="1">'Integrated Register'!$A$3:$V$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Integrated Register'!$A$1:$V$37</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
   <si>
     <t>Status</t>
   </si>
@@ -298,9 +293,6 @@
     <t>Mike</t>
   </si>
   <si>
-    <t>individuals identified in OY3/OY4 will be more aligned with the project</t>
-  </si>
-  <si>
     <t>work being delayed</t>
   </si>
   <si>
@@ -360,6 +352,12 @@
   </si>
   <si>
     <t xml:space="preserve">If HR does not make HR Job Code updates in their system in a timely manner a delay in feed updates will impact time for eCL system updates. </t>
+  </si>
+  <si>
+    <t>individuals identified in OY4 will be more aligned with the project</t>
+  </si>
+  <si>
+    <t>Closed HR related risks - Mike Ingram</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1360,7 +1358,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1574,8 +1572,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>21</v>
@@ -1853,7 +1851,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="7">
         <v>41108</v>
@@ -1862,7 +1860,7 @@
         <v>42551</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>67</v>
@@ -2120,7 +2118,7 @@
         <v>42058</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
@@ -2157,7 +2155,7 @@
       <c r="S10" s="9"/>
       <c r="T10" s="5"/>
       <c r="U10" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V10" s="9"/>
     </row>
@@ -2167,7 +2165,7 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="9">
         <v>41850</v>
@@ -2218,10 +2216,10 @@
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="U11" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="U11" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="V11" s="9"/>
     </row>
@@ -2359,7 +2357,7 @@
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="9">
         <v>42137</v>
@@ -2368,7 +2366,7 @@
         <v>42551</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>59</v>
@@ -2419,11 +2417,11 @@
     </row>
     <row r="15" spans="1:22" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="9">
         <v>42038</v>
@@ -2432,7 +2430,7 @@
         <v>42551</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>67</v>
@@ -2467,27 +2465,27 @@
       </c>
       <c r="P15" s="15"/>
       <c r="Q15" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R15" s="9">
         <v>42403</v>
       </c>
       <c r="S15" s="9"/>
       <c r="T15" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V15" s="9"/>
     </row>
     <row r="16" spans="1:22" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="9">
         <v>42403</v>
@@ -2496,7 +2494,7 @@
         <v>42551</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>86</v>
@@ -2531,17 +2529,17 @@
       </c>
       <c r="P16" s="15"/>
       <c r="Q16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R16" s="9">
         <v>42403</v>
       </c>
       <c r="S16" s="9"/>
       <c r="T16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V16" s="9"/>
     </row>
@@ -3361,10 +3359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3417,7 +3415,7 @@
         <v>42403</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3425,7 +3423,15 @@
         <v>42551</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>42559</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3548,18 +3554,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3579,14 +3585,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3599,4 +3597,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>